<commit_message>
Changed Graphics and added title-Image / demonstartion of my maturaarebeit beeing hidden inside of an image
</commit_message>
<xml_diff>
--- a/Abbildungen - Darstellungen/Farbänderung.xlsx
+++ b/Abbildungen - Darstellungen/Farbänderung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sluz-my.sharepoint.com/personal/samuel_huwiler_sluz_ch/Documents/Desktop/Matura/Auswertung und Abbildungen/Abbildungen - Darstellungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E9B386-5DFD-435A-B620-531842FDD16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{37E9B386-5DFD-435A-B620-531842FDD16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2B8C2B2-70E5-4FCA-B2AF-3008F3644860}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -212,6 +212,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -221,9 +224,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1379,7 +1379,7 @@
   <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1389,16 +1389,16 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:4" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="2:4" ht="84.75" customHeight="1" thickBot="1">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="2:4" ht="21.75" customHeight="1">
       <c r="B4" s="1" t="s">

</xml_diff>